<commit_message>
Dejé funcionando una nueva versión del juego llamada 2.0 en el menú principal con nuevas alternativas de llamados para ejecución de métodos y funciones...
</commit_message>
<xml_diff>
--- a/Precios juegos.xlsx
+++ b/Precios juegos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josue\Documents\NetBeansProjects\poo\JosueGonzalez's World\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36DF538-D8C9-4366-BE79-34FEEA4B2A40}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D15416-251B-47F5-A6E8-7487AFE6006B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" xr2:uid="{F90CFFEC-CC6E-4474-AECE-2BC9BFC24A5F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Precios (recursos) para creación de indumentaria en el juego</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Raza 3 (Esqueletos fantasma)</t>
   </si>
   <si>
-    <t>Recurso 2 (Metal)</t>
-  </si>
-  <si>
-    <t>Recurso 3 (Madera)</t>
-  </si>
-  <si>
     <t>Recurso 2</t>
   </si>
   <si>
@@ -97,6 +91,30 @@
   </si>
   <si>
     <t>&lt;&lt;Coming soon&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Recurso 1 (Arcilla)</t>
+  </si>
+  <si>
+    <t>Recurso 2 (Arena)</t>
+  </si>
+  <si>
+    <t>Recurso 3 (Pedernales)</t>
+  </si>
+  <si>
+    <t>Recurso 2 (Plata)</t>
+  </si>
+  <si>
+    <t>Recurso 1 (Mármol)</t>
+  </si>
+  <si>
+    <t>Recurso 3 (Roble)</t>
+  </si>
+  <si>
+    <t>Recurso 2 (Oro)</t>
+  </si>
+  <si>
+    <t>Recurso 3 (Lava)</t>
   </si>
 </sst>
 </file>
@@ -409,16 +427,162 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -439,9 +603,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -449,140 +610,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,15 +932,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E7F6E1-0030-49FD-BECB-14C4A0D6C697}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19:I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
@@ -918,484 +950,504 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="A5" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9" t="s">
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11" t="s">
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="61"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>5</v>
+      <c r="A7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="6"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="53"/>
-      <c r="G9" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="58"/>
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="48"/>
+      <c r="G9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="50"/>
       <c r="J9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K9">
         <v>3000</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="22">
+      <c r="A10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
         <v>2500</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="5">
         <v>1000</v>
       </c>
-      <c r="D10" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="22">
+      <c r="D10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="5">
         <v>2500</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="10">
         <v>1000</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="22">
+      <c r="G10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="5">
         <v>2500</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="10">
         <v>1000</v>
       </c>
       <c r="J10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K10">
         <v>10000</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="60" t="s">
-        <v>16</v>
+      <c r="A11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="23">
+      <c r="A12" s="6">
         <v>750</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="22">
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5">
         <v>1000</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="8">
         <v>750</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="22">
+      <c r="E12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="5">
         <v>1000</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="9">
         <v>750</v>
       </c>
-      <c r="H12" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="28">
+      <c r="H12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="10">
         <v>1000</v>
       </c>
       <c r="J12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K12">
         <v>5000</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="45"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="47"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="52"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>750</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2000</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8">
+        <v>750</v>
+      </c>
+      <c r="E14" s="5">
+        <v>2000</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="9">
+        <v>750</v>
+      </c>
+      <c r="H14" s="5">
+        <v>2000</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="40"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="32"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="23">
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>500</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1500</v>
+      </c>
+      <c r="C16" s="5">
         <v>750</v>
       </c>
-      <c r="B14" s="22">
-        <v>2000</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="26">
+      <c r="D16" s="8">
+        <v>500</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1500</v>
+      </c>
+      <c r="F16" s="5">
         <v>750</v>
       </c>
-      <c r="E14" s="22">
-        <v>2000</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="27">
+      <c r="G16" s="9">
+        <v>500</v>
+      </c>
+      <c r="H16" s="5">
+        <v>1500</v>
+      </c>
+      <c r="I16" s="10">
         <v>750</v>
       </c>
-      <c r="H14" s="22">
-        <v>2000</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="31" t="s">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
         <v>18</v>
-      </c>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="23">
-        <v>500</v>
-      </c>
-      <c r="B16" s="22">
-        <v>1500</v>
-      </c>
-      <c r="C16" s="22">
-        <v>750</v>
-      </c>
-      <c r="D16" s="26">
-        <v>500</v>
-      </c>
-      <c r="E16" s="22">
-        <v>1500</v>
-      </c>
-      <c r="F16" s="22">
-        <v>750</v>
-      </c>
-      <c r="G16" s="27">
-        <v>500</v>
-      </c>
-      <c r="H16" s="22">
-        <v>1500</v>
-      </c>
-      <c r="I16" s="28">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>20</v>
       </c>
       <c r="B17" s="24"/>
       <c r="C17" s="25"/>
-      <c r="D17" s="34" t="s">
-        <v>20</v>
+      <c r="D17" s="29" t="s">
+        <v>18</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="30"/>
-      <c r="G17" s="31" t="s">
-        <v>20</v>
+      <c r="G17" s="34" t="s">
+        <v>18</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="23">
+      <c r="A18" s="6">
         <v>350</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="5">
         <v>2000</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="5">
         <v>1200</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="8">
         <v>350</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="5">
         <v>2000</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="5">
         <v>1200</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="9">
         <v>350</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="5">
         <v>2000</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="10">
         <v>1200</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="33" t="s">
-        <v>21</v>
+      <c r="A19" s="23" t="s">
+        <v>19</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="25"/>
-      <c r="D19" s="34" t="s">
-        <v>21</v>
+      <c r="D19" s="29" t="s">
+        <v>19</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="30"/>
-      <c r="G19" s="31" t="s">
-        <v>21</v>
+      <c r="G19" s="34" t="s">
+        <v>19</v>
       </c>
       <c r="H19" s="24"/>
       <c r="I19" s="30"/>
-      <c r="J19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
+      <c r="J19" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
     </row>
     <row r="20" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
+      <c r="A20" s="6">
         <v>400</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="5">
         <v>2150</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="5">
         <v>1500</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="8">
         <v>400</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="5">
         <v>2150</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="5">
         <v>1500</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="9">
         <v>400</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="5">
         <v>2150</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="10">
         <v>1500</v>
       </c>
-      <c r="J20" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
+      <c r="J20" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="33" t="s">
-        <v>22</v>
+      <c r="A21" s="23" t="s">
+        <v>20</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="25"/>
-      <c r="D21" s="34" t="s">
-        <v>22</v>
+      <c r="D21" s="29" t="s">
+        <v>20</v>
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="30"/>
-      <c r="G21" s="31" t="s">
-        <v>22</v>
+      <c r="G21" s="34" t="s">
+        <v>20</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="30"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="62"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
-        <v>23</v>
+      <c r="A22" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="25"/>
-      <c r="D22" s="34" t="s">
-        <v>23</v>
+      <c r="D22" s="29" t="s">
+        <v>21</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="30"/>
-      <c r="G22" s="31" t="s">
-        <v>23</v>
+      <c r="G22" s="34" t="s">
+        <v>21</v>
       </c>
       <c r="H22" s="24"/>
       <c r="I22" s="30"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
     </row>
     <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="37"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
     </row>
     <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="62"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M25"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
     <mergeCell ref="A22:C23"/>
     <mergeCell ref="D22:F23"/>
     <mergeCell ref="G22:I23"/>
@@ -1405,26 +1457,6 @@
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M25"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalización de la creación de los métodos a clases restantes, solo queda terminar de llamar los objetos en el menú y agregar las fases
</commit_message>
<xml_diff>
--- a/Precios juegos.xlsx
+++ b/Precios juegos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josue\Documents\NetBeansProjects\poo\JosueGonzalez's World\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D15416-251B-47F5-A6E8-7487AFE6006B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB530BCE-4080-44E0-B6BD-FCD30DEE8F8C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" xr2:uid="{F90CFFEC-CC6E-4474-AECE-2BC9BFC24A5F}"/>
   </bookViews>
@@ -487,134 +487,134 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -933,7 +933,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J15" sqref="J15:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,47 +950,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="57" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="59" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="60"/>
-      <c r="I6" s="61"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
@@ -1036,24 +1036,24 @@
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="47" t="s">
+      <c r="E9" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="48"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="H9" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="50"/>
+      <c r="I9" s="40"/>
       <c r="J9" t="s">
         <v>5</v>
       </c>
@@ -1155,20 +1155,20 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="45"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="47"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="51" t="s">
+      <c r="G13" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="52"/>
+      <c r="H13" s="42"/>
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1201,27 +1201,27 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44" t="s">
+      <c r="E15" s="47"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="40"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="34" t="s">
+      <c r="H15" s="47"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
@@ -1253,21 +1253,21 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="29" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="34" t="s">
+      <c r="E17" s="53"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="30"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="56"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
@@ -1299,27 +1299,27 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="29" t="s">
+      <c r="B19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="34" t="s">
+      <c r="E19" s="53"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="24"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="38" t="s">
+      <c r="H19" s="53"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
     </row>
     <row r="20" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
@@ -1349,90 +1349,93 @@
       <c r="I20" s="10">
         <v>1500</v>
       </c>
-      <c r="J20" s="62" t="s">
+      <c r="J20" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="29" t="s">
+      <c r="B21" s="53"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="34" t="s">
+      <c r="E21" s="53"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="24"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="62"/>
-      <c r="M21" s="62"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="29" t="s">
+      <c r="B22" s="53"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="34" t="s">
+      <c r="E22" s="53"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="24"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="62"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="62"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
     </row>
     <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
     </row>
     <row r="24" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="62"/>
-      <c r="M24" s="62"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="62"/>
-      <c r="M25" s="62"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="D22:F23"/>
+    <mergeCell ref="G22:I23"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
     <mergeCell ref="J19:M19"/>
     <mergeCell ref="J20:M25"/>
     <mergeCell ref="B9:C9"/>
@@ -1449,14 +1452,11 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="A22:C23"/>
-    <mergeCell ref="D22:F23"/>
-    <mergeCell ref="G22:I23"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>